<commit_message>
Updated Add-on Pixel 8x 4 Universes
*. Added support for clock based led chip's (for example APA102)
</commit_message>
<xml_diff>
--- a/Eagle/Addon/Pixel8x4U/CPL.xlsx
+++ b/Eagle/Addon/Pixel8x4U/CPL.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="GD32F207RG" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="GD32F-Pixel8x4U" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -52,6 +52,12 @@
     <t xml:space="preserve">C4</t>
   </si>
   <si>
+    <t xml:space="preserve">C5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6</t>
+  </si>
+  <si>
     <t xml:space="preserve">LED1</t>
   </si>
   <si>
@@ -94,7 +100,40 @@
     <t xml:space="preserve">R11</t>
   </si>
   <si>
+    <t xml:space="preserve">R12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1</t>
+  </si>
+  <si>
     <t xml:space="preserve">U1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2</t>
   </si>
 </sst>
 </file>
@@ -212,14 +251,15 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="5.91"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,16 +284,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>23.18</v>
+        <v>44.45</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>20.96</v>
+        <v>15.24</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -261,16 +301,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>27.3</v>
+        <v>42.23</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>20.96</v>
+        <v>15.24</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -278,16 +318,16 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>36.2</v>
+        <v>33.02</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>16.19</v>
+        <v>14.29</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -295,16 +335,16 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>38.42</v>
+        <v>29.21</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>16.19</v>
+        <v>29.85</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -312,16 +352,16 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>42.23</v>
+        <v>33.02</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>12.38</v>
+        <v>29.85</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>270</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,16 +369,16 @@
         <v>11</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>41.91</v>
+        <v>29.21</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>16.19</v>
+        <v>14.29</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -346,16 +386,16 @@
         <v>12</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>41.91</v>
+        <v>46.04</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>20.64</v>
+        <v>12.7</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -363,16 +403,16 @@
         <v>13</v>
       </c>
       <c r="B9" s="3" t="n">
-        <v>44.77</v>
+        <v>47.31</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>21.59</v>
+        <v>15.24</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -380,16 +420,16 @@
         <v>14</v>
       </c>
       <c r="B10" s="3" t="n">
-        <v>39.05</v>
+        <v>47.31</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>20</v>
+        <v>19.37</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>270</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,16 +437,16 @@
         <v>15</v>
       </c>
       <c r="B11" s="3" t="n">
-        <v>39.05</v>
+        <v>48.9</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>11.75</v>
+        <v>22.54</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -414,16 +454,16 @@
         <v>16</v>
       </c>
       <c r="B12" s="3" t="n">
-        <v>15.88</v>
+        <v>44.77</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>13.34</v>
+        <v>18.73</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -431,16 +471,16 @@
         <v>17</v>
       </c>
       <c r="B13" s="3" t="n">
-        <v>15.88</v>
+        <v>42.86</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>15.88</v>
+        <v>12.7</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -448,16 +488,16 @@
         <v>18</v>
       </c>
       <c r="B14" s="3" t="n">
-        <v>15.88</v>
+        <v>46.99</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>18.41</v>
+        <v>31.75</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -465,10 +505,10 @@
         <v>19</v>
       </c>
       <c r="B15" s="3" t="n">
-        <v>15.88</v>
+        <v>23.18</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>20.96</v>
+        <v>13.97</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>6</v>
@@ -482,10 +522,10 @@
         <v>20</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>15.88</v>
+        <v>23.18</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>29.21</v>
+        <v>15.24</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>6</v>
@@ -499,10 +539,10 @@
         <v>21</v>
       </c>
       <c r="B17" s="3" t="n">
-        <v>15.88</v>
+        <v>23.18</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>31.75</v>
+        <v>16.51</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>6</v>
@@ -516,10 +556,10 @@
         <v>22</v>
       </c>
       <c r="B18" s="3" t="n">
-        <v>15.88</v>
+        <v>23.18</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>34.29</v>
+        <v>17.78</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>6</v>
@@ -533,10 +573,10 @@
         <v>23</v>
       </c>
       <c r="B19" s="3" t="n">
-        <v>15.88</v>
+        <v>23.18</v>
       </c>
       <c r="C19" s="3" t="n">
-        <v>36.83</v>
+        <v>19.05</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>6</v>
@@ -550,108 +590,238 @@
         <v>24</v>
       </c>
       <c r="B20" s="3" t="n">
-        <v>25.4</v>
+        <v>23.18</v>
       </c>
       <c r="C20" s="3" t="n">
-        <v>25.72</v>
+        <v>20.32</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E20" s="3" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="3" t="n">
+        <v>23.18</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>21.59</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>23.18</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>22.86</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="3" t="n">
+        <v>23.18</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>31.43</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>23.18</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>32.7</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="3" t="n">
+        <v>23.18</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>33.97</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>23.18</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>35.24</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="3" t="n">
+        <v>23.18</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>36.51</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>23.18</v>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>37.78</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="3" t="n">
+        <v>23.18</v>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>39.05</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="3" t="n">
+        <v>23.18</v>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>40.32</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>48.9</v>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>38.73</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="3" t="n">
         <v>90</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-    </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="A32" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="3" t="n">
+        <v>31.12</v>
+      </c>
+      <c r="C32" s="3" t="n">
+        <v>19.05</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="3" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="A33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="3" t="n">
+        <v>31.12</v>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>34.93</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="3" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>

</xml_diff>